<commit_message>
cleaned up some UI tried to incorporate python script in MATLAB
</commit_message>
<xml_diff>
--- a/CompletedProgram/Files/Book1.xlsx
+++ b/CompletedProgram/Files/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feroze\Google Drive\DUKE 2016-2020\AxoSim\CompletedProgram\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB3C7577-0A00-4A44-AA7A-9D31187EAF8C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8247E3E8-683B-4061-BC8F-4FA405C2CF5B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5430" xr2:uid="{25BB39F8-F7FB-4861-BC4E-5108884E0129}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>ctrl 1.1.1.txt</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>ctrl 1.2.2.txt</t>
-  </si>
-  <si>
-    <t>ctrl 1.2.3.txt</t>
   </si>
   <si>
     <t>ctrl 1.2.4.txt</t>
@@ -636,13 +633,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E383CDC4-FD42-422E-8570-77797B04C5D8}">
-  <dimension ref="A1:B85"/>
+  <dimension ref="A1:B84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B85"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="20.3671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
@@ -697,7 +697,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>4.235555555555556</v>
+        <v>1.6555555555555554</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -705,7 +705,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1.6555555555555554</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -713,7 +713,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>3.52</v>
+        <v>1.3444444444444446</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -721,7 +721,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1.3444444444444446</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -729,7 +729,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>3.42</v>
+        <v>1.2777777777777777</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -737,7 +737,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1.2777777777777777</v>
+        <v>4.1955555555555559</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -745,7 +745,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>4.1955555555555559</v>
+        <v>1.3822222222222222</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -753,7 +753,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>1.3822222222222222</v>
+        <v>3.88</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -761,7 +761,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>3.88</v>
+        <v>1.2755555555555556</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -769,7 +769,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>1.2755555555555556</v>
+        <v>3.068888888888889</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -777,7 +777,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>3.068888888888889</v>
+        <v>1.3066666666666666</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -785,7 +785,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>1.3066666666666666</v>
+        <v>3.5777777777777779</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -793,7 +793,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>3.5777777777777779</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -801,7 +801,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>1.28</v>
+        <v>3.7466666666666666</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -809,7 +809,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>3.7466666666666666</v>
+        <v>1.2444444444444445</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -817,7 +817,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>1.2444444444444445</v>
+        <v>4.0711111111111107</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -825,7 +825,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>4.0711111111111107</v>
+        <v>1.5266666666666666</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -833,7 +833,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>1.5266666666666666</v>
+        <v>3.0622222222222222</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -841,7 +841,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>3.0622222222222222</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -849,7 +849,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>1.2</v>
+        <v>3.7866666666666666</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -857,7 +857,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>3.7866666666666666</v>
+        <v>1.3511111111111112</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -865,7 +865,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>1.3511111111111112</v>
+        <v>4.0133333333333336</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -873,7 +873,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>4.0133333333333336</v>
+        <v>1.4466666666666668</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -881,7 +881,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>1.4466666666666668</v>
+        <v>3.5933333333333333</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -889,7 +889,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>3.5933333333333333</v>
+        <v>1.3777777777777778</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -897,7 +897,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>1.3777777777777778</v>
+        <v>4.2577777777777781</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -905,7 +905,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>4.2577777777777781</v>
+        <v>1.0955555555555556</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -913,7 +913,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>1.0955555555555556</v>
+        <v>4.2844444444444445</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -921,7 +921,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>4.2844444444444445</v>
+        <v>1.1155555555555556</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -929,7 +929,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>1.1155555555555556</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -937,7 +937,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>4.08</v>
+        <v>3.6155555555555554</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -945,7 +945,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>3.6155555555555554</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -953,7 +953,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>1.1599999999999999</v>
+        <v>3.9777777777777779</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -961,7 +961,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>3.9777777777777779</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -969,7 +969,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>1.1599999999999999</v>
+        <v>3.5511111111111111</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -977,7 +977,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>3.5511111111111111</v>
+        <v>1.2555555555555555</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -985,7 +985,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>1.2555555555555555</v>
+        <v>4.1422222222222222</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -993,7 +993,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>4.1422222222222222</v>
+        <v>1.1933333333333334</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1001,7 +1001,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>1.1933333333333334</v>
+        <v>4.1577777777777776</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1009,7 +1009,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>4.1577777777777776</v>
+        <v>1.3866666666666667</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1017,7 +1017,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>1.3866666666666667</v>
+        <v>4.0866666666666669</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1025,7 +1025,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>4.0866666666666669</v>
+        <v>1.4488888888888889</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1033,7 +1033,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>1.4488888888888889</v>
+        <v>4.12</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1041,7 +1041,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>4.12</v>
+        <v>1.7066666666666668</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1049,7 +1049,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>1.7066666666666668</v>
+        <v>3.7111111111111112</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1057,7 +1057,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>3.7111111111111112</v>
+        <v>1.0777777777777777</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1065,7 +1065,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>1.0777777777777777</v>
+        <v>3.5466666666666669</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1073,7 +1073,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>3.5466666666666669</v>
+        <v>1.0644444444444445</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1081,7 +1081,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>1.0644444444444445</v>
+        <v>4.24</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1089,7 +1089,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>4.24</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1097,7 +1097,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>1.52</v>
+        <v>3.82</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1105,7 +1105,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>3.82</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1113,7 +1113,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>1.4</v>
+        <v>4.2733333333333334</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1121,7 +1121,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>4.2733333333333334</v>
+        <v>1.4044444444444444</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1129,7 +1129,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>1.4044444444444444</v>
+        <v>3.7422222222222223</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1137,7 +1137,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>3.7422222222222223</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1145,7 +1145,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>1.38</v>
+        <v>3.7044444444444444</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1153,7 +1153,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>3.7044444444444444</v>
+        <v>1.1288888888888888</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1161,7 +1161,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>1.1288888888888888</v>
+        <v>1.2288888888888889</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1169,7 +1169,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>1.2288888888888889</v>
+        <v>4.5733333333333333</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1177,7 +1177,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>4.5733333333333333</v>
+        <v>1.2622222222222221</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1185,7 +1185,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>1.2622222222222221</v>
+        <v>4.6977777777777776</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1193,7 +1193,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>4.6977777777777776</v>
+        <v>3.9155555555555557</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1201,7 +1201,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>3.9155555555555557</v>
+        <v>0.96666666666666667</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1209,7 +1209,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>0.96666666666666667</v>
+        <v>4.4444444444444446</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1217,7 +1217,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>4.4444444444444446</v>
+        <v>1.3111111111111111</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1225,7 +1225,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>1.3111111111111111</v>
+        <v>3.7155555555555555</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1233,7 +1233,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>3.7155555555555555</v>
+        <v>1.2066666666666668</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1241,7 +1241,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>1.2066666666666668</v>
+        <v>3.7266666666666666</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1249,7 +1249,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>3.7266666666666666</v>
+        <v>1.048888888888889</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1257,7 +1257,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>1.048888888888889</v>
+        <v>3.5333333333333332</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1265,7 +1265,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>3.5333333333333332</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1273,7 +1273,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>1.22</v>
+        <v>3.34</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1281,7 +1281,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>3.34</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1289,7 +1289,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>1.1599999999999999</v>
+        <v>4.0777777777777775</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1297,7 +1297,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>4.0777777777777775</v>
+        <v>1.3133333333333332</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1305,7 +1305,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>1.3133333333333332</v>
+        <v>4.3177777777777777</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1313,14 +1313,6 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>4.3177777777777777</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" t="s">
-        <v>84</v>
-      </c>
-      <c r="B85">
         <v>1.4622222222222223</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added presentation images and final presentation
</commit_message>
<xml_diff>
--- a/CompletedProgram/Files/Book1.xlsx
+++ b/CompletedProgram/Files/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feroze\Google Drive\DUKE 2016-2020\AxoSim\CompletedProgram\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEDC657-25D2-4961-9888-76F08232FC81}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908FAAC4-0F9F-4940-9341-AE7253C12AEC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5430" xr2:uid="{25BB39F8-F7FB-4861-BC4E-5108884E0129}"/>
   </bookViews>
@@ -30,15 +30,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>ctrl 1.1.1.txt</t>
   </si>
   <si>
     <t>ctrl 1.1.2.txt</t>
-  </si>
-  <si>
-    <t>ctrl 1.1.3.txt</t>
   </si>
   <si>
     <t>ctrl 1.1.4.txt</t>
@@ -636,7 +633,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E383CDC4-FD42-422E-8570-77797B04C5D8}">
-  <dimension ref="A1:B85"/>
+  <dimension ref="A1:B84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -668,7 +665,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>3.1066666666666665</v>
+        <v>1.1022222222222222</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -676,23 +673,23 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1.1022222222222222</v>
+        <v>3.6222222222222222</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="B5">
-        <v>3.6222222222222222</v>
+        <v>4.235555555555556</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>4.235555555555556</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -700,7 +697,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1.1599999999999999</v>
+        <v>1.6555555555555554</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -708,7 +705,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1.6555555555555554</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -716,7 +713,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>3.52</v>
+        <v>1.3444444444444446</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -724,7 +721,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1.3444444444444446</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -732,7 +729,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>3.42</v>
+        <v>1.2777777777777777</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -740,7 +737,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1.2777777777777777</v>
+        <v>4.1955555555555559</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -748,7 +745,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>4.1955555555555559</v>
+        <v>1.3822222222222222</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -756,7 +753,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>1.3822222222222222</v>
+        <v>3.88</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -764,7 +761,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>3.88</v>
+        <v>1.2755555555555556</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -772,7 +769,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>1.2755555555555556</v>
+        <v>3.068888888888889</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -780,7 +777,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>3.068888888888889</v>
+        <v>1.3066666666666666</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -788,7 +785,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>1.3066666666666666</v>
+        <v>3.5777777777777779</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -796,7 +793,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>3.5777777777777779</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -804,7 +801,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1.28</v>
+        <v>3.7466666666666666</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -812,7 +809,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>3.7466666666666666</v>
+        <v>1.2444444444444445</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -820,7 +817,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1.2444444444444445</v>
+        <v>4.0711111111111107</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -828,7 +825,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>4.0711111111111107</v>
+        <v>1.5266666666666666</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -836,7 +833,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>1.5266666666666666</v>
+        <v>3.0622222222222222</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -844,7 +841,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>3.0622222222222222</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -852,7 +849,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1.2</v>
+        <v>3.7866666666666666</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -860,7 +857,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>3.7866666666666666</v>
+        <v>1.3511111111111112</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -868,7 +865,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>1.3511111111111112</v>
+        <v>4.0133333333333336</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -876,7 +873,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>4.0133333333333336</v>
+        <v>1.4466666666666668</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -884,7 +881,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>1.4466666666666668</v>
+        <v>3.5933333333333333</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -892,7 +889,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>3.5933333333333333</v>
+        <v>1.3777777777777778</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -900,7 +897,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>1.3777777777777778</v>
+        <v>4.2577777777777781</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -908,7 +905,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>4.2577777777777781</v>
+        <v>1.0955555555555556</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -916,7 +913,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>1.0955555555555556</v>
+        <v>4.2844444444444445</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -924,7 +921,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>4.2844444444444445</v>
+        <v>1.1155555555555556</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -932,7 +929,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>1.1155555555555556</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -940,7 +937,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>4.08</v>
+        <v>3.6155555555555554</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -948,7 +945,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>3.6155555555555554</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -956,7 +953,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>1.1599999999999999</v>
+        <v>3.9777777777777779</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -964,7 +961,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>3.9777777777777779</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -972,7 +969,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>1.1599999999999999</v>
+        <v>3.5511111111111111</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -980,7 +977,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>3.5511111111111111</v>
+        <v>1.2555555555555555</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -988,7 +985,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>1.2555555555555555</v>
+        <v>4.1422222222222222</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -996,7 +993,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>4.1422222222222222</v>
+        <v>1.1933333333333334</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1004,7 +1001,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>1.1933333333333334</v>
+        <v>4.1577777777777776</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1012,7 +1009,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>4.1577777777777776</v>
+        <v>1.3866666666666667</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1020,7 +1017,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>1.3866666666666667</v>
+        <v>4.0866666666666669</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1028,7 +1025,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>4.0866666666666669</v>
+        <v>1.4488888888888889</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1036,7 +1033,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>1.4488888888888889</v>
+        <v>4.12</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1044,7 +1041,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>4.12</v>
+        <v>1.7066666666666668</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1052,7 +1049,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>1.7066666666666668</v>
+        <v>3.7111111111111112</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1060,7 +1057,7 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>3.7111111111111112</v>
+        <v>1.0777777777777777</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1068,7 +1065,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>1.0777777777777777</v>
+        <v>3.5466666666666669</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1076,7 +1073,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>3.5466666666666669</v>
+        <v>1.0644444444444445</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1084,7 +1081,7 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>1.0644444444444445</v>
+        <v>4.24</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1092,7 +1089,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>4.24</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1100,7 +1097,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>1.52</v>
+        <v>3.82</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1108,7 +1105,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>3.82</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1116,7 +1113,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>1.4</v>
+        <v>4.2733333333333334</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1124,7 +1121,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>4.2733333333333334</v>
+        <v>1.4044444444444444</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1132,7 +1129,7 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>1.4044444444444444</v>
+        <v>3.7422222222222223</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1140,7 +1137,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>3.7422222222222223</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1148,7 +1145,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>1.38</v>
+        <v>3.7044444444444444</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1156,7 +1153,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>3.7044444444444444</v>
+        <v>1.1288888888888888</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1164,7 +1161,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>1.1288888888888888</v>
+        <v>1.2288888888888889</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1172,7 +1169,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>1.2288888888888889</v>
+        <v>4.5733333333333333</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1180,7 +1177,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>4.5733333333333333</v>
+        <v>1.2622222222222221</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1188,7 +1185,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>1.2622222222222221</v>
+        <v>4.6977777777777776</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1196,7 +1193,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>4.6977777777777776</v>
+        <v>3.9155555555555557</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1204,7 +1201,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>3.9155555555555557</v>
+        <v>0.96666666666666667</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1212,7 +1209,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0.96666666666666667</v>
+        <v>4.4444444444444446</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1220,7 +1217,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>4.4444444444444446</v>
+        <v>1.3111111111111111</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1228,7 +1225,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>1.3111111111111111</v>
+        <v>3.7155555555555555</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1236,7 +1233,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>3.7155555555555555</v>
+        <v>1.2066666666666668</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1244,7 +1241,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>1.2066666666666668</v>
+        <v>3.7266666666666666</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1252,7 +1249,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>3.7266666666666666</v>
+        <v>1.048888888888889</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1260,7 +1257,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>1.048888888888889</v>
+        <v>3.5333333333333332</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1268,7 +1265,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>3.5333333333333332</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1276,7 +1273,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>1.22</v>
+        <v>3.34</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1284,7 +1281,7 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>3.34</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1292,7 +1289,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>1.1599999999999999</v>
+        <v>4.0777777777777775</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1300,7 +1297,7 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>4.0777777777777775</v>
+        <v>1.3133333333333332</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1308,7 +1305,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>1.3133333333333332</v>
+        <v>4.3177777777777777</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1316,14 +1313,6 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>4.3177777777777777</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" t="s">
-        <v>83</v>
-      </c>
-      <c r="B85">
         <v>1.4622222222222223</v>
       </c>
     </row>

</xml_diff>